<commit_message>
Major optimisation to dataUpload
</commit_message>
<xml_diff>
--- a/SAMPLE_DATA/xlsx/timetable.xlsx
+++ b/SAMPLE_DATA/xlsx/timetable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pranav\Timetable_Manager_Backend\src\sampleData\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Organized\Projects\timetable_manager\SAMPLE_DATA\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA0952A-2C18-4C4A-8642-6587BE6B8E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B8A211-6E57-43CF-B23D-D1A5118C6131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B4273205-B7A3-4DF5-B3CB-DDE6D75C5AFA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="53">
   <si>
     <t>batch_name</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>CL 02</t>
+  </si>
+  <si>
+    <t>Basic French I</t>
   </si>
 </sst>
 </file>
@@ -262,14 +265,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,15 +450,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{86E301DE-6AE7-46E0-9FAB-F8402CEB83BC}" name="Table1" displayName="Table1" ref="A1:I100" totalsRowShown="0" dataDxfId="9">
-  <autoFilter ref="A1:I100" xr:uid="{86E301DE-6AE7-46E0-9FAB-F8402CEB83BC}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="a1"/>
-        <filter val="a2"/>
-        <filter val="a3"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I100" xr:uid="{86E301DE-6AE7-46E0-9FAB-F8402CEB83BC}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I91">
     <sortCondition ref="A1:A91"/>
   </sortState>
@@ -796,8 +788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD2615D8-1A23-494F-8DF7-113148D5E742}">
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="D91" sqref="D91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -851,7 +843,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>40</v>
@@ -876,7 +868,7 @@
         <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>40</v>
@@ -901,7 +893,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>40</v>
@@ -915,7 +907,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -940,7 +932,7 @@
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -965,7 +957,7 @@
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -990,7 +982,7 @@
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1015,7 +1007,7 @@
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1040,7 +1032,7 @@
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1140,7 +1132,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>9</v>
       </c>
@@ -1165,7 +1157,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1190,7 +1182,7 @@
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
@@ -1215,7 +1207,7 @@
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1240,7 +1232,7 @@
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -1265,7 +1257,7 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1365,7 +1357,7 @@
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1390,7 +1382,7 @@
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1415,7 +1407,7 @@
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1440,7 +1432,7 @@
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>9</v>
       </c>
@@ -1465,7 +1457,7 @@
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1490,7 +1482,7 @@
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1590,7 +1582,7 @@
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1615,7 +1607,7 @@
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>9</v>
       </c>
@@ -1640,7 +1632,7 @@
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1657,7 @@
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1690,7 +1682,7 @@
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1707,7 @@
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1815,7 +1807,7 @@
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
@@ -1840,7 +1832,7 @@
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -1865,7 +1857,7 @@
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>9</v>
       </c>
@@ -1890,7 +1882,7 @@
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>9</v>
       </c>
@@ -1915,7 +1907,7 @@
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -1940,7 +1932,7 @@
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>9</v>
       </c>
@@ -2040,7 +2032,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -2065,7 +2057,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>9</v>
       </c>
@@ -2090,7 +2082,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2107,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>9</v>
       </c>
@@ -2140,7 +2132,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>9</v>
       </c>
@@ -2165,7 +2157,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
@@ -2265,7 +2257,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>9</v>
       </c>
@@ -2290,7 +2282,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>9</v>
       </c>
@@ -2315,7 +2307,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>9</v>
       </c>
@@ -2340,7 +2332,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>9</v>
       </c>
@@ -2365,7 +2357,7 @@
       <c r="H62" s="1"/>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>9</v>
       </c>
@@ -2390,7 +2382,7 @@
       <c r="H63" s="1"/>
       <c r="I63" s="1"/>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>9</v>
       </c>
@@ -2490,7 +2482,7 @@
       <c r="H67" s="1"/>
       <c r="I67" s="1"/>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>9</v>
       </c>
@@ -2515,7 +2507,7 @@
       <c r="H68" s="1"/>
       <c r="I68" s="1"/>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>9</v>
       </c>
@@ -2540,7 +2532,7 @@
       <c r="H69" s="1"/>
       <c r="I69" s="1"/>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>9</v>
       </c>
@@ -2565,7 +2557,7 @@
       <c r="H70" s="1"/>
       <c r="I70" s="1"/>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
@@ -2590,7 +2582,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>9</v>
       </c>
@@ -2615,7 +2607,7 @@
       <c r="H72" s="1"/>
       <c r="I72" s="1"/>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>9</v>
       </c>
@@ -2715,7 +2707,7 @@
       <c r="H76" s="1"/>
       <c r="I76" s="1"/>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>9</v>
       </c>
@@ -2740,7 +2732,7 @@
       <c r="H77" s="1"/>
       <c r="I77" s="1"/>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>9</v>
       </c>
@@ -2765,7 +2757,7 @@
       <c r="H78" s="1"/>
       <c r="I78" s="1"/>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>9</v>
       </c>
@@ -2790,7 +2782,7 @@
       <c r="H79" s="1"/>
       <c r="I79" s="1"/>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>9</v>
       </c>
@@ -2815,7 +2807,7 @@
       <c r="H80" s="1"/>
       <c r="I80" s="1"/>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>9</v>
       </c>
@@ -2840,7 +2832,7 @@
       <c r="H81" s="1"/>
       <c r="I81" s="1"/>
     </row>
-    <row r="82" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>9</v>
       </c>
@@ -2940,7 +2932,7 @@
       <c r="H85" s="1"/>
       <c r="I85" s="1"/>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>9</v>
       </c>
@@ -2965,7 +2957,7 @@
       <c r="H86" s="1"/>
       <c r="I86" s="1"/>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>9</v>
       </c>
@@ -2990,7 +2982,7 @@
       <c r="H87" s="1"/>
       <c r="I87" s="1"/>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>9</v>
       </c>
@@ -3015,7 +3007,7 @@
       <c r="H88" s="1"/>
       <c r="I88" s="1"/>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>9</v>
       </c>
@@ -3040,7 +3032,7 @@
       <c r="H89" s="1"/>
       <c r="I89" s="1"/>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>9</v>
       </c>
@@ -3065,7 +3057,7 @@
       <c r="H90" s="1"/>
       <c r="I90" s="1"/>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>9</v>
       </c>
@@ -3091,229 +3083,229 @@
       <c r="I91" s="3"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B92" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C92" s="4" t="s">
+      <c r="A92" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D92" s="4" t="s">
+      <c r="D92" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E92" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F92" s="4" t="s">
+      <c r="E92" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G92" s="5" t="s">
+      <c r="G92" t="s">
         <v>51</v>
       </c>
-      <c r="H92" s="4"/>
-      <c r="I92" s="4"/>
+      <c r="H92" s="1"/>
+      <c r="I92" s="1"/>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C93" s="4" t="s">
+      <c r="A93" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D93" s="4" t="s">
+      <c r="D93" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E93" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F93" s="4" t="s">
+      <c r="E93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G93" s="5" t="s">
+      <c r="G93" t="s">
         <v>51</v>
       </c>
-      <c r="H93" s="4"/>
-      <c r="I93" s="4"/>
+      <c r="H93" s="1"/>
+      <c r="I93" s="1"/>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C94" s="4" t="s">
+      <c r="A94" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D94" s="4" t="s">
+      <c r="D94" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E94" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F94" s="4" t="s">
+      <c r="E94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G94" s="5" t="s">
+      <c r="G94" t="s">
         <v>51</v>
       </c>
-      <c r="H94" s="4"/>
-      <c r="I94" s="4"/>
-    </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C95" s="4" t="s">
+      <c r="H94" s="1"/>
+      <c r="I94" s="1"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D95" s="4" t="s">
+      <c r="D95" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E95" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F95" s="4" t="s">
+      <c r="E95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F95" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G95" s="5" t="s">
+      <c r="G95" t="s">
         <v>51</v>
       </c>
-      <c r="H95" s="4"/>
-      <c r="I95" s="4"/>
-    </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C96" s="4" t="s">
+      <c r="H95" s="1"/>
+      <c r="I95" s="1"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D96" s="4" t="s">
+      <c r="D96" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E96" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F96" s="4" t="s">
+      <c r="E96" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F96" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G96" s="5" t="s">
+      <c r="G96" t="s">
         <v>51</v>
       </c>
-      <c r="H96" s="4"/>
-      <c r="I96" s="4"/>
-    </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B97" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C97" s="4" t="s">
+      <c r="H96" s="1"/>
+      <c r="I96" s="1"/>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D97" s="4" t="s">
+      <c r="D97" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E97" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F97" s="4" t="s">
+      <c r="E97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F97" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G97" s="5" t="s">
+      <c r="G97" t="s">
         <v>51</v>
       </c>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
-    </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B98" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C98" s="4" t="s">
+      <c r="H97" s="1"/>
+      <c r="I97" s="1"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E98" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F98" s="4" t="s">
+      <c r="E98" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F98" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G98" s="5" t="s">
+      <c r="G98" t="s">
         <v>51</v>
       </c>
-      <c r="H98" s="4"/>
-      <c r="I98" s="4"/>
-    </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B99" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C99" s="4" t="s">
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D99" s="4" t="s">
+      <c r="D99" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E99" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F99" s="4" t="s">
+      <c r="E99" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F99" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G99" s="5" t="s">
+      <c r="G99" t="s">
         <v>51</v>
       </c>
-      <c r="H99" s="4"/>
-      <c r="I99" s="4"/>
-    </row>
-    <row r="100" spans="1:9" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B100" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C100" s="6" t="s">
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+    </row>
+    <row r="100" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D100" s="6" t="s">
+      <c r="D100" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E100" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F100" s="6" t="s">
+      <c r="E100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F100" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G100" s="5" t="s">
+      <c r="G100" t="s">
         <v>51</v>
       </c>
-      <c r="H100" s="6"/>
-      <c r="I100" s="6"/>
+      <c r="H100" s="3"/>
+      <c r="I100" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>